<commit_message>
actualizamos archivos y borramos otros
</commit_message>
<xml_diff>
--- a/servicios/output_datos/tabla_padron_actualizado.xlsx
+++ b/servicios/output_datos/tabla_padron_actualizado.xlsx
@@ -2542,8 +2542,8 @@
   </sheetPr>
   <dimension ref="A1:AM196"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="T1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="X1" activeCellId="0" sqref="X1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2779,7 +2779,7 @@
         <v>42</v>
       </c>
       <c r="X2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y2" s="0" t="s">
         <v>44</v>
@@ -3017,7 +3017,7 @@
         <v>42</v>
       </c>
       <c r="X4" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y4" s="0" t="s">
         <v>60</v>
@@ -3124,7 +3124,7 @@
         <v>48</v>
       </c>
       <c r="T5" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U5" s="0" t="s">
         <v>68</v>
@@ -3136,7 +3136,7 @@
         <v>21972</v>
       </c>
       <c r="X5" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y5" s="0" t="s">
         <v>70</v>
@@ -3255,7 +3255,7 @@
         <v>42</v>
       </c>
       <c r="X6" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y6" s="0" t="s">
         <v>72</v>
@@ -3374,7 +3374,7 @@
         <v>42</v>
       </c>
       <c r="X7" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y7" s="0" t="s">
         <v>77</v>
@@ -3731,7 +3731,7 @@
         <v>42</v>
       </c>
       <c r="X10" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y10" s="0" t="s">
         <v>88</v>
@@ -3850,7 +3850,7 @@
         <v>42</v>
       </c>
       <c r="X11" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y11" s="0" t="s">
         <v>93</v>
@@ -4088,7 +4088,7 @@
         <v>42</v>
       </c>
       <c r="X13" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y13" s="0" t="s">
         <v>108</v>
@@ -4314,7 +4314,7 @@
         <v>48</v>
       </c>
       <c r="T15" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U15" s="0" t="s">
         <v>125</v>
@@ -4326,7 +4326,7 @@
         <v>24764</v>
       </c>
       <c r="X15" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y15" s="0" t="s">
         <v>127</v>
@@ -4445,7 +4445,7 @@
         <v>42</v>
       </c>
       <c r="X16" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y16" s="0" t="s">
         <v>133</v>
@@ -4564,7 +4564,7 @@
         <v>54</v>
       </c>
       <c r="X17" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y17" s="0" t="s">
         <v>142</v>
@@ -4671,7 +4671,7 @@
         <v>48</v>
       </c>
       <c r="T18" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U18" s="0" t="s">
         <v>151</v>
@@ -4683,7 +4683,7 @@
         <v>23620</v>
       </c>
       <c r="X18" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y18" s="0" t="s">
         <v>153</v>
@@ -4790,7 +4790,7 @@
         <v>48</v>
       </c>
       <c r="T19" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U19" s="0" t="s">
         <v>160</v>
@@ -5278,7 +5278,7 @@
         <v>42</v>
       </c>
       <c r="X23" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y23" s="0" t="s">
         <v>185</v>
@@ -5397,7 +5397,7 @@
         <v>42</v>
       </c>
       <c r="X24" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y24" s="0" t="s">
         <v>193</v>
@@ -5516,7 +5516,7 @@
         <v>42</v>
       </c>
       <c r="X25" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y25" s="0" t="s">
         <v>199</v>
@@ -5635,7 +5635,7 @@
         <v>42</v>
       </c>
       <c r="X26" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y26" s="0" t="s">
         <v>208</v>
@@ -5754,7 +5754,7 @@
         <v>42</v>
       </c>
       <c r="X27" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y27" s="0" t="s">
         <v>216</v>
@@ -5873,7 +5873,7 @@
         <v>42</v>
       </c>
       <c r="X28" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y28" s="0" t="s">
         <v>221</v>
@@ -6337,7 +6337,7 @@
         <v>48</v>
       </c>
       <c r="T32" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U32" s="0" t="s">
         <v>243</v>
@@ -6349,7 +6349,7 @@
         <v>32262</v>
       </c>
       <c r="X32" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y32" s="0" t="s">
         <v>245</v>
@@ -6456,7 +6456,7 @@
         <v>48</v>
       </c>
       <c r="T33" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U33" s="0" t="s">
         <v>251</v>
@@ -6468,7 +6468,7 @@
         <v>30861</v>
       </c>
       <c r="X33" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y33" s="0" t="s">
         <v>253</v>
@@ -6575,7 +6575,7 @@
         <v>48</v>
       </c>
       <c r="T34" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U34" s="0" t="s">
         <v>260</v>
@@ -6694,7 +6694,7 @@
         <v>48</v>
       </c>
       <c r="T35" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U35" s="0" t="s">
         <v>268</v>
@@ -6706,7 +6706,7 @@
         <v>30010</v>
       </c>
       <c r="X35" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y35" s="0" t="s">
         <v>269</v>
@@ -6825,7 +6825,7 @@
         <v>42</v>
       </c>
       <c r="X36" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y36" s="0" t="s">
         <v>276</v>
@@ -6944,7 +6944,7 @@
         <v>42</v>
       </c>
       <c r="X37" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y37" s="0" t="s">
         <v>282</v>
@@ -7182,7 +7182,7 @@
         <v>42</v>
       </c>
       <c r="X39" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y39" s="0" t="s">
         <v>291</v>
@@ -7301,7 +7301,7 @@
         <v>42</v>
       </c>
       <c r="X40" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y40" s="0" t="s">
         <v>296</v>
@@ -7539,7 +7539,7 @@
         <v>42</v>
       </c>
       <c r="X42" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y42" s="0" t="s">
         <v>305</v>
@@ -8253,7 +8253,7 @@
         <v>42</v>
       </c>
       <c r="X48" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y48" s="0" t="s">
         <v>323</v>
@@ -8372,7 +8372,7 @@
         <v>42</v>
       </c>
       <c r="X49" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y49" s="0" t="s">
         <v>327</v>
@@ -8729,7 +8729,7 @@
         <v>42</v>
       </c>
       <c r="X52" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y52" s="0" t="s">
         <v>336</v>
@@ -8848,7 +8848,7 @@
         <v>42</v>
       </c>
       <c r="X53" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y53" s="0" t="s">
         <v>345</v>
@@ -9086,7 +9086,7 @@
         <v>42</v>
       </c>
       <c r="X55" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y55" s="0" t="s">
         <v>355</v>
@@ -9443,7 +9443,7 @@
         <v>42</v>
       </c>
       <c r="X58" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y58" s="0" t="s">
         <v>365</v>
@@ -9800,7 +9800,7 @@
         <v>42</v>
       </c>
       <c r="X61" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y61" s="0" t="s">
         <v>375</v>
@@ -9919,7 +9919,7 @@
         <v>42</v>
       </c>
       <c r="X62" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y62" s="0" t="s">
         <v>377</v>
@@ -10157,7 +10157,7 @@
         <v>42</v>
       </c>
       <c r="X64" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y64" s="0" t="s">
         <v>386</v>
@@ -10276,7 +10276,7 @@
         <v>42</v>
       </c>
       <c r="X65" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y65" s="0" t="s">
         <v>391</v>
@@ -10395,7 +10395,7 @@
         <v>42</v>
       </c>
       <c r="X66" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y66" s="0" t="s">
         <v>396</v>
@@ -10514,7 +10514,7 @@
         <v>42</v>
       </c>
       <c r="X67" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y67" s="0" t="s">
         <v>400</v>
@@ -10633,7 +10633,7 @@
         <v>42</v>
       </c>
       <c r="X68" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y68" s="0" t="s">
         <v>403</v>
@@ -10871,7 +10871,7 @@
         <v>42</v>
       </c>
       <c r="X70" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y70" s="0" t="s">
         <v>410</v>
@@ -11347,7 +11347,7 @@
         <v>42</v>
       </c>
       <c r="X74" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y74" s="0" t="s">
         <v>425</v>
@@ -11585,7 +11585,7 @@
         <v>42</v>
       </c>
       <c r="X76" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y76" s="0" t="s">
         <v>433</v>
@@ -11704,7 +11704,7 @@
         <v>42</v>
       </c>
       <c r="X77" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y77" s="0" t="s">
         <v>437</v>
@@ -11823,7 +11823,7 @@
         <v>42</v>
       </c>
       <c r="X78" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y78" s="0" t="s">
         <v>441</v>
@@ -12180,7 +12180,7 @@
         <v>42</v>
       </c>
       <c r="X81" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y81" s="0" t="s">
         <v>451</v>
@@ -12299,7 +12299,7 @@
         <v>42</v>
       </c>
       <c r="X82" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y82" s="0" t="s">
         <v>455</v>
@@ -12656,7 +12656,7 @@
         <v>42</v>
       </c>
       <c r="X85" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y85" s="0" t="s">
         <v>465</v>
@@ -13251,7 +13251,7 @@
         <v>42</v>
       </c>
       <c r="X90" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y90" s="0" t="s">
         <v>484</v>
@@ -13370,7 +13370,7 @@
         <v>42</v>
       </c>
       <c r="X91" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y91" s="0" t="s">
         <v>488</v>
@@ -13846,7 +13846,7 @@
         <v>42</v>
       </c>
       <c r="X95" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y95" s="0" t="s">
         <v>497</v>
@@ -14203,7 +14203,7 @@
         <v>42</v>
       </c>
       <c r="X98" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y98" s="0" t="s">
         <v>506</v>
@@ -14560,7 +14560,7 @@
         <v>42</v>
       </c>
       <c r="X101" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y101" s="0" t="s">
         <v>516</v>
@@ -14679,7 +14679,7 @@
         <v>42</v>
       </c>
       <c r="X102" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y102" s="0" t="s">
         <v>520</v>
@@ -14798,7 +14798,7 @@
         <v>42</v>
       </c>
       <c r="X103" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y103" s="0" t="s">
         <v>525</v>
@@ -14917,7 +14917,7 @@
         <v>42</v>
       </c>
       <c r="X104" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y104" s="0" t="s">
         <v>529</v>
@@ -15036,7 +15036,7 @@
         <v>42</v>
       </c>
       <c r="X105" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y105" s="0" t="s">
         <v>534</v>
@@ -15274,7 +15274,7 @@
         <v>42</v>
       </c>
       <c r="X107" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y107" s="0" t="s">
         <v>542</v>
@@ -15393,7 +15393,7 @@
         <v>42</v>
       </c>
       <c r="X108" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y108" s="0" t="s">
         <v>546</v>
@@ -15512,7 +15512,7 @@
         <v>42</v>
       </c>
       <c r="X109" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y109" s="0" t="s">
         <v>550</v>
@@ -15869,7 +15869,7 @@
         <v>42</v>
       </c>
       <c r="X112" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y112" s="0" t="s">
         <v>563</v>
@@ -16107,7 +16107,7 @@
         <v>42</v>
       </c>
       <c r="X114" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y114" s="0" t="s">
         <v>570</v>
@@ -16583,7 +16583,7 @@
         <v>42</v>
       </c>
       <c r="X118" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y118" s="0" t="s">
         <v>583</v>
@@ -16702,7 +16702,7 @@
         <v>42</v>
       </c>
       <c r="X119" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y119" s="0" t="s">
         <v>588</v>
@@ -16821,7 +16821,7 @@
         <v>42</v>
       </c>
       <c r="X120" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y120" s="0" t="s">
         <v>592</v>
@@ -17297,7 +17297,7 @@
         <v>42</v>
       </c>
       <c r="X124" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y124" s="0" t="s">
         <v>608</v>
@@ -17416,7 +17416,7 @@
         <v>42</v>
       </c>
       <c r="X125" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y125" s="0" t="s">
         <v>612</v>
@@ -17654,7 +17654,7 @@
         <v>42</v>
       </c>
       <c r="X127" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y127" s="0" t="s">
         <v>620</v>
@@ -17773,7 +17773,7 @@
         <v>42</v>
       </c>
       <c r="X128" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y128" s="0" t="s">
         <v>626</v>
@@ -17892,7 +17892,7 @@
         <v>42</v>
       </c>
       <c r="X129" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y129" s="0" t="s">
         <v>630</v>
@@ -18487,7 +18487,7 @@
         <v>42</v>
       </c>
       <c r="X134" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y134" s="0" t="s">
         <v>644</v>
@@ -18725,7 +18725,7 @@
         <v>42</v>
       </c>
       <c r="X136" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y136" s="0" t="s">
         <v>652</v>
@@ -18963,7 +18963,7 @@
         <v>42</v>
       </c>
       <c r="X138" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y138" s="0" t="s">
         <v>659</v>
@@ -21343,7 +21343,7 @@
         <v>42</v>
       </c>
       <c r="X158" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y158" s="0" t="s">
         <v>695</v>
@@ -25615,7 +25615,7 @@
         <v>275</v>
       </c>
       <c r="T194" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U194" s="0" t="s">
         <v>695</v>

</xml_diff>